<commit_message>
Atualização da validação do import excel com os novos campos
</commit_message>
<xml_diff>
--- a/static/downloads/ArquivoModelo.xlsx
+++ b/static/downloads/ArquivoModelo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernandororato/Documents/F5Sys/OrionTax/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernandororato/Documents/F5Sys/OrionTax/integrador_CICD/static/downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C3E0448-F5E8-1545-A422-CC7E51B48655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922FF0A7-35D4-EC4C-ACD2-24E77FDB262E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27320" windowHeight="13680" xr2:uid="{DC56A3F7-1372-7F4B-9487-4A8ABF7C6C26}"/>
+    <workbookView xWindow="3920" yWindow="500" windowWidth="23400" windowHeight="13680" xr2:uid="{DC56A3F7-1372-7F4B-9487-4A8ABF7C6C26}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>codigo</t>
   </si>
@@ -125,6 +125,24 @@
   </si>
   <si>
     <t>7896331100136</t>
+  </si>
+  <si>
+    <t>tipo_produto</t>
+  </si>
+  <si>
+    <t>outros_detalhes</t>
+  </si>
+  <si>
+    <t>Insumos</t>
+  </si>
+  <si>
+    <t>Imobilizado</t>
+  </si>
+  <si>
+    <t>Revenda</t>
+  </si>
+  <si>
+    <t>sem detalhes</t>
   </si>
 </sst>
 </file>
@@ -485,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A38D8912-6596-9F44-B68D-3BD270B4A931}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -508,9 +526,11 @@
     <col min="13" max="13" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -556,8 +576,14 @@
       <c r="O1" t="s">
         <v>14</v>
       </c>
+      <c r="P1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -597,8 +623,11 @@
       <c r="O2" s="1">
         <v>116</v>
       </c>
+      <c r="P2" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -638,8 +667,11 @@
       <c r="O3" s="1">
         <v>116</v>
       </c>
+      <c r="P3" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -682,8 +714,14 @@
       <c r="O4" s="1">
         <v>0</v>
       </c>
+      <c r="P4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="5" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -726,8 +764,11 @@
       <c r="O5" s="1">
         <v>0</v>
       </c>
+      <c r="P5" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="6" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>6</v>
       </c>
@@ -770,8 +811,11 @@
       <c r="O6" s="1">
         <v>110</v>
       </c>
+      <c r="P6" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="7" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>7</v>
       </c>
@@ -816,6 +860,9 @@
       </c>
       <c r="O7" s="1">
         <v>126</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>